<commit_message>
Added note for CH:VAT to 0183
</commit_message>
<xml_diff>
--- a/current/PEPPOL Code List - Participant Identifier Issuing Agencies 4.0 DRAFT.xlsx
+++ b/current/PEPPOL Code List - Participant Identifier Issuing Agencies 4.0 DRAFT.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Participant" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Participant!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Participant!$A$1:$I$68</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="251">
   <si>
     <t>GLN</t>
   </si>
@@ -849,6 +849,9 @@
       </rPr>
       <t>9.999.999.999 - Check: 99 = 97 - (9.999.999.9 modulo 97)</t>
     </r>
+  </si>
+  <si>
+    <t>Auch CID 183</t>
   </si>
 </sst>
 </file>
@@ -1362,11 +1365,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,7 +1829,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -1865,7 +1869,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1939,7 +1943,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -2047,7 +2051,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>115</v>
       </c>
@@ -2064,7 +2068,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>116</v>
       </c>
@@ -2081,7 +2085,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>117</v>
       </c>
@@ -2098,7 +2102,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>118</v>
       </c>
@@ -2115,7 +2119,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>119</v>
       </c>
@@ -2132,7 +2136,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>120</v>
       </c>
@@ -2148,8 +2152,11 @@
       <c r="E38" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>183</v>
       </c>
@@ -2166,7 +2173,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>121</v>
       </c>
@@ -2183,7 +2190,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>122</v>
       </c>
@@ -2200,7 +2207,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>123</v>
       </c>
@@ -2217,7 +2224,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>212</v>
       </c>
@@ -2234,7 +2241,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>124</v>
       </c>
@@ -2251,7 +2258,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>125</v>
       </c>
@@ -2268,7 +2275,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>126</v>
       </c>
@@ -2285,7 +2292,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>127</v>
       </c>
@@ -2302,7 +2309,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>128</v>
       </c>
@@ -2666,10 +2673,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1">
-    <sortState ref="A2:C26">
-      <sortCondition ref="B1"/>
-    </sortState>
+  <autoFilter ref="A1:I68">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="false"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>